<commit_message>
Implemented and debugged CheckManageFile(), CheckTranslocFile() and started to work on ReadManageFile()
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TranslocationFile.xlsx
+++ b/doc/Manual/Batchmode/TranslocationFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreeg.IBB\eclipse-workspace\RangeShifter_transloc\doc\Manual\Batchmode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreeg.IBB\RangeShiftR\transloc_new_genetics_spatial_demog\RangeShifter_batch\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC8568F-C0FE-49BB-BCC2-26BC6D80808B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314A02F1-5256-4069-9F6A-EE794A5C5949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Simulation</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>SourcePatchID</t>
-  </si>
-  <si>
-    <t>TargetPatchID</t>
-  </si>
-  <si>
     <t>MaxAge</t>
   </si>
   <si>
@@ -68,12 +62,6 @@
     <t>Patch_ID or X and Y location of the source location from which individuals are catched.</t>
   </si>
   <si>
-    <t>SourcePatchID OR SourceX and SourceY</t>
-  </si>
-  <si>
-    <t>TargetPatchID OR SourceX and SourceY</t>
-  </si>
-  <si>
     <t>Patch_ID or X and Y location of the target location from which individuals are catched.</t>
   </si>
   <si>
@@ -96,6 +84,15 @@
   </si>
   <si>
     <t>Sex of the individual to be translocated: Only for sexual models, otherwise set to -9 to ignore</t>
+  </si>
+  <si>
+    <t>Integer value or semicolon seperated integer values (cell-based)</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -540,21 +537,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -565,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -576,205 +573,205 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C28"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45"/>
     </row>
   </sheetData>
@@ -786,24 +783,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,28 +808,28 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C3" s="2"/>
     </row>
   </sheetData>

</xml_diff>